<commit_message>
Revisión Guía Rápida Financiamiento y Obligaciones
</commit_message>
<xml_diff>
--- a/PDRMYE/ENTREGABLES/Matriz de Puebas/Matiz de Pruebas PDRMYE DAMOP.xlsx
+++ b/PDRMYE/ENTREGABLES/Matriz de Puebas/Matiz de Pruebas PDRMYE DAMOP.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INAP-QA\Documents\GITHUB\All-documents-\PDRMYE\ENTREGABLES\Matriz de Puebas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\github\All-documents\PDRMYE\ENTREGABLES\Matriz de Puebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="106">
   <si>
     <t xml:space="preserve">Matriz de Pruebas </t>
   </si>
@@ -422,6 +422,15 @@
   </si>
   <si>
     <t xml:space="preserve">Se pueden ocultar columnas ajustando el tamaño de la tabla. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuentas Bancarias </t>
+  </si>
+  <si>
+    <t>Agredar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filtros </t>
   </si>
 </sst>
 </file>
@@ -11244,8 +11253,8 @@
   <dimension ref="A1:N355"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O14" sqref="O14"/>
+      <pane ySplit="6" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -12705,52 +12714,157 @@
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="8:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B49" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" t="s">
+        <v>103</v>
+      </c>
+      <c r="D49" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" t="s">
+        <v>22</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="H49"/>
     </row>
-    <row r="50" spans="8:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B50" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" t="s">
+        <v>103</v>
+      </c>
+      <c r="D50" t="s">
+        <v>21</v>
+      </c>
+      <c r="E50" t="s">
+        <v>22</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="H50"/>
     </row>
-    <row r="51" spans="8:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B51" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" t="s">
+        <v>103</v>
+      </c>
+      <c r="D51" t="s">
+        <v>21</v>
+      </c>
+      <c r="E51" t="s">
+        <v>22</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="N51" s="1"/>
     </row>
-    <row r="52" spans="8:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B52" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" t="s">
+        <v>103</v>
+      </c>
+      <c r="D52" t="s">
+        <v>21</v>
+      </c>
+      <c r="E52" t="s">
+        <v>22</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="N52" s="1"/>
     </row>
-    <row r="53" spans="8:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B53" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" t="s">
+        <v>103</v>
+      </c>
+      <c r="D53" t="s">
+        <v>21</v>
+      </c>
+      <c r="E53" t="s">
+        <v>22</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="N53" s="1"/>
     </row>
-    <row r="54" spans="8:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B54" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" t="s">
+        <v>103</v>
+      </c>
+      <c r="D54" t="s">
+        <v>21</v>
+      </c>
+      <c r="E54" t="s">
+        <v>22</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="N54" s="1"/>
     </row>
-    <row r="55" spans="8:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B55" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" t="s">
+        <v>103</v>
+      </c>
+      <c r="D55" t="s">
+        <v>21</v>
+      </c>
+      <c r="E55" t="s">
+        <v>22</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="N55" s="1"/>
     </row>
-    <row r="56" spans="8:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:14" x14ac:dyDescent="0.3">
       <c r="N56" s="1"/>
     </row>
-    <row r="57" spans="8:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:14" x14ac:dyDescent="0.3">
       <c r="N57" s="1"/>
     </row>
-    <row r="58" spans="8:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:14" x14ac:dyDescent="0.3">
       <c r="N58" s="1"/>
     </row>
-    <row r="59" spans="8:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:14" x14ac:dyDescent="0.3">
       <c r="N59" s="1"/>
     </row>
-    <row r="60" spans="8:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.3">
       <c r="N60" s="1"/>
     </row>
-    <row r="61" spans="8:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:14" x14ac:dyDescent="0.3">
       <c r="N61" s="1"/>
     </row>
-    <row r="62" spans="8:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:14" x14ac:dyDescent="0.3">
       <c r="N62" s="1"/>
     </row>
-    <row r="63" spans="8:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:14" x14ac:dyDescent="0.3">
       <c r="N63" s="1"/>
     </row>
-    <row r="64" spans="8:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:14" x14ac:dyDescent="0.3">
       <c r="N64" s="1"/>
     </row>
     <row r="65" spans="14:14" x14ac:dyDescent="0.3">

</xml_diff>